<commit_message>
Integrate Agora data for elec/BDPbES, elec/BDSBaPCF, elec/BRPSPTY, and trans/BNVFE
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9373152E-02BF-429E-84B0-76634958027A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="38880" yWindow="3840" windowWidth="13635" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Notes:</t>
   </si>
@@ -61,15 +73,6 @@
     <t>for purposes of guaranteed dispatch.</t>
   </si>
   <si>
-    <t>We assign priority 1 to natural gas peaker and petroleum-fired plants, which are the</t>
-  </si>
-  <si>
-    <t>for the United States.  We arbitrarily assign priority 2 to all other plant types.</t>
-  </si>
-  <si>
-    <t>only types for which a non-zero quantity is specified for guaranteed dispatch in the BAU case</t>
-  </si>
-  <si>
     <t>lignite</t>
   </si>
   <si>
@@ -93,11 +96,17 @@
   <si>
     <t>Priority Order (dimensionless)</t>
   </si>
+  <si>
+    <t xml:space="preserve">We assign priority 2 to all of them as the merit-order is in place in the EU 28. </t>
+  </si>
+  <si>
+    <t>Even though there are support schemes for certain types we assume market-based dispatch according to least marginal cost.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,6 +246,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -272,6 +298,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,46 +490,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -496,23 +536,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2">
         <v>2015</v>
@@ -623,9 +665,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -771,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -919,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1215,9 +1257,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1363,7 +1405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1511,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1807,7 +1849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1955,305 +1997,305 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2399,9 +2441,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2547,9 +2589,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2695,9 +2737,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2843,9 +2885,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>2</v>

</xml_diff>

<commit_message>
Uploading Agora/EI elec, endo-learn, and fuels data files
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27021"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05002382-202A-4BFB-9F71-B62C33F79EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9373152E-02BF-429E-84B0-76634958027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38880" yWindow="3840" windowWidth="13635" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +37,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>BDPbES BAU Dispatch Priority by Electricity Source</t>
+  </si>
   <si>
     <t>Notes:</t>
   </si>
@@ -42,10 +48,31 @@
     <t>This variable is used to specify the priority ordering of the different electricity sources</t>
   </si>
   <si>
+    <t>for purposes of guaranteed dispatch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We assign priority 2 to all of them as the merit-order is in place in the EU 28. </t>
+  </si>
+  <si>
+    <t>Even though there are support schemes for certain types we assume market-based dispatch according to least marginal cost.</t>
+  </si>
+  <si>
+    <t>Priority Order (dimensionless)</t>
+  </si>
+  <si>
+    <t>hard coal</t>
+  </si>
+  <si>
+    <t>natural gas nonpeaker</t>
+  </si>
+  <si>
     <t>nuclear</t>
   </si>
   <si>
     <t>hydro</t>
+  </si>
+  <si>
+    <t>onshore wind</t>
   </si>
   <si>
     <t>solar PV</t>
@@ -57,12 +84,6 @@
     <t>biomass</t>
   </si>
   <si>
-    <t>BDPbES BAU Dispatch Priority by Electricity Source</t>
-  </si>
-  <si>
-    <t>natural gas nonpeaker</t>
-  </si>
-  <si>
     <t>geothermal</t>
   </si>
   <si>
@@ -72,25 +93,7 @@
     <t>natural gas peaker</t>
   </si>
   <si>
-    <t>for purposes of guaranteed dispatch.</t>
-  </si>
-  <si>
-    <t>We assign priority 1 to natural gas peaker and petroleum-fired plants, which are the</t>
-  </si>
-  <si>
-    <t>for the United States.  We arbitrarily assign priority 2 to all other plant types.</t>
-  </si>
-  <si>
-    <t>only types for which a non-zero quantity is specified for guaranteed dispatch in the BAU case</t>
-  </si>
-  <si>
     <t>lignite</t>
-  </si>
-  <si>
-    <t>hard coal</t>
-  </si>
-  <si>
-    <t>onshore wind</t>
   </si>
   <si>
     <t>offshore wind</t>
@@ -104,36 +107,12 @@
   <si>
     <t>municipal solid waste</t>
   </si>
-  <si>
-    <t>Priority Order (dimensionless)</t>
-  </si>
-  <si>
-    <t>hard coal w CCS</t>
-  </si>
-  <si>
-    <t>natural gas combined cycle w CCS</t>
-  </si>
-  <si>
-    <t>biomass w CCS</t>
-  </si>
-  <si>
-    <t>lignite w CCS</t>
-  </si>
-  <si>
-    <t>small modular reactor</t>
-  </si>
-  <si>
-    <t>hydrogen combustion turbine</t>
-  </si>
-  <si>
-    <t>hydrogen combined cycle</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,13 +124,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,12 +158,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,45 +462,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -545,21 +511,21 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK24"/>
+  <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:AK24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="28.5">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2">
         <v>2015</v>
@@ -670,9 +636,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -818,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -966,9 +932,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1114,9 +1080,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1262,9 +1228,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1410,9 +1376,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1558,9 +1524,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1706,9 +1672,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1854,9 +1820,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2002,305 +1968,305 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2446,7 +2412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2594,7 +2560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2602,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:R24" si="3">$B15</f>
+        <f t="shared" ref="C15:C17" si="3">$B15</f>
         <v>2</v>
       </c>
       <c r="D15">
@@ -2742,7 +2708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2890,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2962,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="S17">
-        <f t="shared" ref="S17:AK18" si="4">$B17</f>
+        <f t="shared" ref="S17:AK17" si="4">$B17</f>
         <v>2</v>
       </c>
       <c r="T17">
@@ -3035,1046 +3001,265 @@
       </c>
       <c r="AK17">
         <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="X18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Y18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AA18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AC18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AD18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AE18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AF18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AG18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AH18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AI18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AJ18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AK18">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ref="D19:AK24" si="5">$B19</f>
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="T24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="W24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="X24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AB24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AC24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ24">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK24">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDEE9883-8851-495D-B431-F0FA878F4452}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65B1A20A-F3F4-4362-93A5-06D01B0B8AD4}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{050708E1-63EB-42D9-ABD0-4ABE3CF80F25}"/>
 </file>
</xml_diff>